<commit_message>
Ajustes backend relatórios, NotificatorWhatsapp, KeysCustom
</commit_message>
<xml_diff>
--- a/templates/export/route.xlsx
+++ b/templates/export/route.xlsx
@@ -1,44 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Автор</author>
+    <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>jx:area(lastCell="H9")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,11 +29,11 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>jx:each(items="devices", var="device", lastCell="H9" multisheet="sheetNames")</t>
+          <t>jx:area(lastCell="E9")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0" shapeId="0">
+    <comment ref="A3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -62,7 +43,21 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>jx:each(items="device.objects", var="position", lastCell="H9")</t>
+          <t>jx:each(items="devices", var="device", lastCell="E9" multisheet="sheetNames")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>jx:each(items="device.objects", var="position", lastCell="E9")</t>
         </r>
       </text>
     </comment>
@@ -71,33 +66,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>Report type:</t>
-  </si>
-  <si>
-    <t>Route</t>
-  </si>
-  <si>
-    <t>Device:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>${device.deviceName}</t>
   </si>
   <si>
-    <t>Group:</t>
-  </si>
-  <si>
-    <t>${device.groupName}</t>
-  </si>
-  <si>
-    <t>Period:</t>
-  </si>
-  <si>
-    <t>Valid</t>
-  </si>
-  <si>
-    <t>Time</t>
+    <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", from, locale, timezone)+" - "+dateTool.format("YYYY-MM-dd HH:mm:ss", to, locale, timezone)}</t>
+  </si>
+  <si>
+    <t>Relatório de Rotas</t>
+  </si>
+  <si>
+    <t>Periodo</t>
+  </si>
+  <si>
+    <t>Veiculo</t>
   </si>
   <si>
     <t>Latitude</t>
@@ -106,19 +89,7 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>Altitude</t>
-  </si>
-  <si>
-    <t>Speed</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Attributes</t>
-  </si>
-  <si>
-    <t>${position.valid}</t>
+    <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", position.fixTime, locale, timezone)}</t>
   </si>
   <si>
     <t>${position.latitude}</t>
@@ -127,34 +98,30 @@
     <t>${position.longitude}</t>
   </si>
   <si>
-    <t>${position.altitude}</t>
-  </si>
-  <si>
     <t>${speedUnit.equals("kmh") ? "".format("%.1f km/h", position.speed * 1.852) : speedUnit.equals("mph") ? "".format("%.1f mph", position.speed * 1.15078) : "".format("%.1f kn", position.speed)}</t>
   </si>
   <si>
-    <t>${position.attributes.toString().replaceAll(",", " ").replaceAll(bracketsRegex, "")}</t>
-  </si>
-  <si>
-    <t>${util.hyperlink("".format("https://www.openstreetmap.org/?mlat=%1$f&amp;mlon=%2$f#map=16/%1$f/%2$f", position.latitude, position.longitude), position.getAddress() == null ? "".format("%1$f°, %2$f°", position.latitude, position.longitude) : position.address)}</t>
-  </si>
-  <si>
-    <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", from, locale, timezone)+" - "+dateTool.format("YYYY-MM-dd HH:mm:ss", to, locale, timezone)}</t>
-  </si>
-  <si>
-    <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", position.fixTime, locale, timezone)}</t>
+    <t>Horario</t>
+  </si>
+  <si>
+    <t>Velocidade</t>
+  </si>
+  <si>
+    <t>Endereço</t>
+  </si>
+  <si>
+    <t>${util.hyperlink("".format("https://google.com/maps/place/%1$f,%2$f", position.latitude, position.longitude), position.getAddress() == null ? "".format("%1$f°, %2$f°", position.latitude, position.longitude) : position.address)}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
-    <numFmt numFmtId="166" formatCode="0&quot; m&quot;"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -164,6 +131,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF444444"/>
       <name val="Calibri"/>
@@ -186,20 +160,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -208,8 +168,9 @@
       <charset val="204"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -222,28 +183,29 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,6 +215,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF5B9BD5"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF585570"/>
         <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
@@ -281,69 +249,73 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="15"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Пояснение" xfId="1" builtinId="53" customBuiltin="1"/>
+  <cellStyles count="7">
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="1"/>
+    <cellStyle name="Explanatory Text 2" xfId="2"/>
+    <cellStyle name="Explanatory Text 3" xfId="3"/>
+    <cellStyle name="Explanatory Text 4" xfId="4"/>
+    <cellStyle name="Explanatory Text 5" xfId="5"/>
+    <cellStyle name="Explanatory Text 6" xfId="6"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -364,14 +336,14 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF7F7F7F"/>
       <rgbColor rgb="FF5B9BD5"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0070C0"/>
+      <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -415,14 +387,6 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -436,10 +400,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4019040</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>275730</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>180525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -449,7 +413,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11381760" cy="9524520"/>
+          <a:ext cx="12565800" cy="9524520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -487,10 +451,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4019040</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>275730</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>180525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -500,7 +464,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11381760" cy="9524520"/>
+          <a:ext cx="12565800" cy="9524520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -538,10 +502,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4019040</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>275730</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>180525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -551,7 +515,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11381760" cy="9524520"/>
+          <a:ext cx="12565800" cy="9524520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -589,22 +553,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4019550</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1133280</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1030" name="shapetype_202" hidden="1"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
+        <xdr:cNvPr id="5" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
+          <a:ext cx="10013400" cy="9524520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -616,11 +578,21 @@
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
+          <a:miter/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -632,22 +604,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4019550</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1133280</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
+        <xdr:cNvPr id="6" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
+          <a:ext cx="10013400" cy="9524520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -659,11 +629,21 @@
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
+          <a:miter/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -675,22 +655,20 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4019550</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1133280</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
+        <xdr:cNvPr id="7" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
+          <a:ext cx="10013400" cy="9524520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -702,11 +680,21 @@
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
+          <a:miter/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -714,9 +702,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -724,39 +712,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -788,10 +776,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -823,10 +810,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -835,306 +821,284 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375"/>
-    <col min="2" max="2" width="20.7109375"/>
-    <col min="3" max="4" width="13"/>
-    <col min="5" max="5" width="10.7109375"/>
-    <col min="6" max="6" width="11.42578125"/>
-    <col min="7" max="7" width="61.85546875"/>
-    <col min="8" max="8" width="73.28515625"/>
-    <col min="9" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="57.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+    <row r="2" spans="1:5" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4"/>
+    <row r="3" spans="1:5" ht="26.25">
+      <c r="A3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>3</v>
-      </c>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
+      <c r="B5" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="4"/>
+      <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" ht="29.25" customHeight="1">
+      <c r="A8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="4"/>
+      <c r="D8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+    <row r="9" spans="1:5" ht="21.75" customHeight="1">
+      <c r="A9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="11" t="s">
+      <c r="E9" s="9" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="B6:C6"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>

</xml_diff>